<commit_message>
Upgrade knowledge base and adjust layouts
Adds come skills to quick reply on knowledge base and
some adjusts in the css and html.
</commit_message>
<xml_diff>
--- a/knowledge/corona_qa.xlsx
+++ b/knowledge/corona_qa.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="96">
   <si>
     <t xml:space="preserve">Pergunta</t>
   </si>
@@ -165,7 +165,59 @@
     <t xml:space="preserve">O que causa o corona de onde surgiu origem do corona virus</t>
   </si>
   <si>
-    <t xml:space="preserve">Esses vírus receberam esse nome devido às espículas na sua superfície que lembram uma coroa. Existem quatro grupos principais de coronavírus: alfa, beta, gama, e delta.  Os primeiros coronavírus humanos foram inicialmente identificados em meados da década de 1960. Os seis coronavírus que infectam humanos são: alpha coronavírus 229E e NL63, beta coronavírus OC43 e HKU1, SARS-CoV (coronavírus causador da Síndrome Respiratória Aguda Grave ou SARS), e MERS-CoV (novo coronavírus causador da Síndrome Respiratória do Oriente Médio ou MERS).  Existem vários coronavírus que infectam naturalmente animais. A maioria destes geralmente infecta somente uma espécie animal, ou no máximo, um pequeno número de espécies proximamente relacionadas. Porém, SARS-CoV infecta tanto humanos como outros animais, incluindo macacos, civetes, guaxinim, gatos, cachorros e roedores. MERS-CoV também foi encontrado infectando humanos e animais, incluindo camelos e morcegos.</t>
+    <t xml:space="preserve">Esses vírus receberam esse nome devido às espículas na sua superfície que lembram uma coroa. Existem quatro grupos principais de coronavírus: alfa, beta, gama, e delta.  Os primeiros coronavírus humanos foram inicialmente identificados em meados da década de 1960. Os seis coronavírus que infectam humanos são: alpha coronavírus 229E e NL63, beta coronavírus OC43 e HKU1, SARS-CoV (coronavírus causador da Síndrome Respiratória Aguda Grave ou SARS), e MERS-CoV (novo coronavírus causador da Síndrome Respiratória do Oriente Médio ou MERS).  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SARS-CoV detalhes tecnicos técnicos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Existem vários coronavírus que infectam naturalmente animais. A maioria destes geralmente infecta somente uma espécie animal, ou no máximo, um pequeno número de espécies proximamente relacionadas. Porém, SARS-CoV infecta tanto humanos como outros animais, incluindo macacos, civetes, guaxinim, gatos, cachorros e roedores. MERS-CoV também foi encontrado infectando humanos e animais, incluindo camelos e morcegos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Como devo lavar as mãos como lavar as mãos lavar mao mãos corretamente higienizar as mãos higiene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passe sabonete e água limpa nas mãos&lt;br&gt;  Esfregue a palma de cada mão&lt;br&gt; Esfregue a ponta dos dedos na palma da outra mão&lt;br&gt; Esfregue entre os dedos de cada mão&lt;br&gt;Esfregue o polegar de cada mão&lt;br&gt;Lave o dorso de cada mão&lt;br&gt; Lave os punhos de ambas as mãos&lt;br&gt; Seque com uma toalha limpa ou papel toalha.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.youtube.com/embed/rsQlyIwetsE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Como se previnir Como previnir o corona prevenção como não ser infectado evitar o corona</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Lave as mãos com água e sabão ou use álcool em gel&lt;br&gt; Cubra o nariz e boca ao espirrar ou tossir&lt;br&gt;Evite aglomerações se estiver doente&lt;br&gt;Mantenha os ambientes bem ventilados</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">&lt;br&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Não compartilhe objetos pessoais. </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.youtube.com/embed/eKRwSN5SUko</t>
   </si>
   <si>
     <t xml:space="preserve">O que se entende por “lucro real” e “lucro tributável”?</t>
@@ -333,12 +385,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF72BF44"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -382,7 +440,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -404,6 +462,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -486,7 +556,7 @@
       <rgbColor rgb="FFFFC7CE"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF72BF44"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFC55A11"/>
@@ -773,25 +843,26 @@
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="66.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.53"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2"/>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="7" t="s">
         <v>42</v>
       </c>
     </row>
@@ -816,10 +887,44 @@
       <c r="B3" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="8" t="s">
         <v>47</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -842,6 +947,8 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="https://www.youtube.com/embed/BA9NE59SV_o"/>
+    <hyperlink ref="D5" r:id="rId2" display="https://www.youtube.com/embed/rsQlyIwetsE"/>
+    <hyperlink ref="D6" r:id="rId3" display="https://www.youtube.com/embed/eKRwSN5SUko"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
@@ -887,10 +994,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -898,10 +1005,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -909,10 +1016,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -920,10 +1027,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -931,10 +1038,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -942,10 +1049,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -953,10 +1060,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -964,10 +1071,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -975,10 +1082,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -986,10 +1093,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -997,10 +1104,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1008,10 +1115,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1019,10 +1126,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1030,10 +1137,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1041,10 +1148,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1052,10 +1159,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1063,10 +1170,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1074,10 +1181,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1085,10 +1192,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1096,10 +1203,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes folders structures and updates readme
</commit_message>
<xml_diff>
--- a/knowledge/corona_qa.xlsx
+++ b/knowledge/corona_qa.xlsx
@@ -186,35 +186,7 @@
     <t xml:space="preserve">Como se previnir Como previnir o corona prevenção como não ser infectado evitar o corona</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Lave as mãos com água e sabão ou use álcool em gel&lt;br&gt; Cubra o nariz e boca ao espirrar ou tossir&lt;br&gt;Evite aglomerações se estiver doente&lt;br&gt;Mantenha os ambientes bem ventilados</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">&lt;br&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Não compartilhe objetos pessoais. </t>
-    </r>
+    <t xml:space="preserve">Lave as mãos com água e sabão ou use álcool em gel&lt;br&gt; Cubra o nariz e boca ao espirrar ou tossir&lt;br&gt;Evite aglomerações se estiver doente&lt;br&gt;Mantenha os ambientes bem ventilados&lt;br&gt;Não compartilhe objetos pessoais. </t>
   </si>
   <si>
     <t xml:space="preserve">https://www.youtube.com/embed/eKRwSN5SUko</t>
@@ -347,7 +319,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -377,12 +349,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -440,7 +406,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -474,10 +440,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -843,7 +805,7 @@
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -866,7 +828,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
         <v>1</v>
       </c>
@@ -892,10 +854,10 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finishes conversation and upgrade knowledge
Now, when user finishes a conversation, bot
returns to initial state.
Upgrade xls file with some news skills.
</commit_message>
<xml_diff>
--- a/knowledge/corona_qa.xlsx
+++ b/knowledge/corona_qa.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="104">
   <si>
     <t xml:space="preserve">Pergunta</t>
   </si>
@@ -190,6 +190,30 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.youtube.com/embed/eKRwSN5SUko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Como o coronavírus é transmitido?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As investigações sobre as formas de transmissão do coronavírus ainda estão em andamento, mas a disseminação de pessoa para pessoa, ou seja, a contaminação por gotículas respiratórias ou contato, está ocorrendo. &lt;br /&gt; Qualquer pessoa que tenha contato próximo (cerca de 1m) com alguém com sintomas respiratórios está em risco de ser exposta à infecção. &lt;br /&gt; É importante observar que a disseminação de pessoa para pessoa pode ocorrer de forma continuada. &lt;br /&gt; Alguns vírus são altamente contagiosos (como sarampo), enquanto outros são menos. Ainda não está claro com que facilidade o coronavírus se espalha de pessoa para pessoa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quais as formas de transmissão? Como  transmite Como pegar Transmissão</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> gotículas de saliva; &lt;br /&gt; &lt;br /&gt;espirro; &lt;br /&gt; &lt;br /&gt;tosse; &lt;br /&gt; &lt;br /&gt;catarro; &lt;br /&gt; &lt;br /&gt;contato pessoal próximo, como toque ou aperto de mão; &lt;br /&gt; &lt;br /&gt;contato com objetos ou superfícies contaminadas, seguido de contato com a boca, nariz ou olhos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qual o período de incubação ? Tempo de recuperação incubação Quanto demora para recuperar Quantos dias fico em casa Quantos dias para curar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O período médio de incubação por coronavírus é de 5 dias, com intervalos que chegam a 12 dias, período em que os primeiros sintomas levam para aparecer desde a infecção.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qual o tratamento? Tratamento remédio como curar tratamento cura tempo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Não existe tratamento específico para infecções causadas por coronavírus humano. No caso do coronavírus é indicado repouso e consumo de bastante água, além de algumas medidas adotadas para aliviar os sintomas, conforme cada caso, como, por exemplo: &lt;br /&gt; Uso de medicamento para dor e febre (antitérmicos e analgésicos). &lt;br /&gt; Uso de umidificador no quarto ou tomar banho quente para auxiliar no alívio da dor de garanta e tosse. &lt;br /&gt; Assim que os primeiros sintomas surgirem, é fundamental procurar ajuda médica imediata para confirmar diagnóstico e iniciar o tratamento. &lt;br /&gt; Todos os pacientes que receberem alta durante os primeiros 07 dias do início do quadro (qualquer sintoma independente de febre), devem ser alertados para a possibilidade de piora tardia do quadro clínico e sinais de alerta de complicações como: aparecimento de febre (podendo haver casos iniciais sem febre), elevação ou reaparecimento de febre ou sinais respiratórios, taquicardia (aumento dos batimentos cardíacos), dor pleurítica (dor no peito), fadiga (cansaço) e dispnéia (falta de ar).</t>
   </si>
   <si>
     <t xml:space="preserve">O que se entende por “lucro real” e “lucro tributável”?</t>
@@ -805,7 +829,7 @@
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -883,10 +907,38 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
     <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -956,10 +1008,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -967,10 +1019,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -978,10 +1030,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -989,10 +1041,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1000,10 +1052,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1011,10 +1063,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1022,10 +1074,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1033,10 +1085,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1044,10 +1096,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1055,10 +1107,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1066,10 +1118,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1077,10 +1129,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1088,10 +1140,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1099,10 +1151,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1110,10 +1162,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1121,10 +1173,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1132,10 +1184,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1143,10 +1195,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1154,10 +1206,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1165,10 +1217,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>